<commit_message>
dynamic prediction: working model
</commit_message>
<xml_diff>
--- a/ISA Encoding.xlsx
+++ b/ISA Encoding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Logic Design Projects\risc-v-32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E48FDF3-F956-4086-B671-1C77708C958C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED89AF3-0815-4BC0-A33D-E0DDE29B7008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0864E286-8FD9-4BCF-9303-3B3C9A244ACA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0864E286-8FD9-4BCF-9303-3B3C9A244ACA}"/>
   </bookViews>
   <sheets>
     <sheet name="ISA Encoding" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="139">
   <si>
     <t>BEQ</t>
   </si>
@@ -441,13 +441,16 @@
     <t>lhu rd, ra, offset</t>
   </si>
   <si>
-    <t>sb ra, rb, offset</t>
-  </si>
-  <si>
-    <t>sh ra, rb, offset</t>
-  </si>
-  <si>
     <t>JAL</t>
+  </si>
+  <si>
+    <t>sb rb, ra, offset</t>
+  </si>
+  <si>
+    <t>sh rb, ra, offset</t>
+  </si>
+  <si>
+    <t>sw rb, ra, offset</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -539,6 +542,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -857,9 +863,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AB332B-A77B-4F57-9E6E-188FD1D08F1A}">
   <dimension ref="A1:AV50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AR3" sqref="AR3:AR7"/>
+      <selection pane="topRight" activeCell="AV50" sqref="AV50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,29 +1023,29 @@
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
       <c r="S2" s="1">
         <v>0</v>
       </c>
@@ -1049,32 +1055,32 @@
       <c r="U2" s="1">
         <v>0</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="V2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="12">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="12">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="12">
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="14">
         <v>1</v>
       </c>
       <c r="AI2" s="13" t="s">
@@ -1100,23 +1106,23 @@
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
       <c r="S3" s="1">
         <v>0</v>
       </c>
@@ -1126,18 +1132,18 @@
       <c r="U3" s="1">
         <v>1</v>
       </c>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
       <c r="AI3" s="13"/>
       <c r="AM3" s="10" t="s">
         <v>73</v>
@@ -1159,23 +1165,23 @@
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
       <c r="S4" s="1">
         <v>1</v>
       </c>
@@ -1185,18 +1191,18 @@
       <c r="U4" s="1">
         <v>0</v>
       </c>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="12"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="14"/>
       <c r="AI4" s="13"/>
       <c r="AM4" s="10" t="s">
         <v>73</v>
@@ -1218,23 +1224,23 @@
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
       <c r="S5" s="1">
         <v>1</v>
       </c>
@@ -1244,18 +1250,18 @@
       <c r="U5" s="1">
         <v>1</v>
       </c>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
       <c r="AI5" s="13"/>
       <c r="AM5" s="10" t="s">
         <v>73</v>
@@ -1277,23 +1283,23 @@
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
       <c r="S6" s="1">
         <v>1</v>
       </c>
@@ -1303,18 +1309,18 @@
       <c r="U6" s="1">
         <v>0</v>
       </c>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="12"/>
-      <c r="AC6" s="12"/>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="14"/>
       <c r="AI6" s="13"/>
       <c r="AM6" s="10" t="s">
         <v>73</v>
@@ -1336,23 +1342,23 @@
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
       <c r="S7" s="1">
         <v>1</v>
       </c>
@@ -1362,18 +1368,18 @@
       <c r="U7" s="1">
         <v>1</v>
       </c>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
-      <c r="AA7" s="12"/>
-      <c r="AB7" s="12"/>
-      <c r="AC7" s="12"/>
-      <c r="AD7" s="12"/>
-      <c r="AE7" s="12"/>
-      <c r="AF7" s="12"/>
-      <c r="AG7" s="12"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="14"/>
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="14"/>
       <c r="AI7" s="13"/>
       <c r="AM7" s="10" t="s">
         <v>73</v>
@@ -1395,27 +1401,27 @@
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
       <c r="S8" s="1">
         <v>0</v>
       </c>
@@ -1425,13 +1431,13 @@
       <c r="U8" s="1">
         <v>0</v>
       </c>
-      <c r="V8" s="12" t="s">
+      <c r="V8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="12"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
       <c r="AA8" s="1">
         <v>1</v>
       </c>
@@ -1480,35 +1486,35 @@
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="12"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
       <c r="AA9" s="1">
         <v>1</v>
       </c>
@@ -1559,33 +1565,33 @@
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="12"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
       <c r="AA10" s="1">
         <v>0</v>
       </c>
@@ -1633,31 +1639,31 @@
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
       <c r="AA11" s="1">
         <v>0</v>
       </c>
@@ -1700,27 +1706,27 @@
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
       <c r="S12" s="1">
         <v>0</v>
       </c>
@@ -1730,30 +1736,30 @@
       <c r="U12" s="1">
         <v>0</v>
       </c>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="12"/>
-      <c r="AA12" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="12">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="12">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG12" s="12">
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="14">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="14">
         <v>1</v>
       </c>
       <c r="AI12" s="13" t="s">
@@ -1797,19 +1803,19 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
       <c r="S13" s="1">
         <v>0</v>
       </c>
@@ -1819,18 +1825,18 @@
       <c r="U13" s="1">
         <v>1</v>
       </c>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="12"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="12"/>
-      <c r="AE13" s="12"/>
-      <c r="AF13" s="12"/>
-      <c r="AG13" s="12"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="14"/>
+      <c r="AG13" s="14"/>
       <c r="AI13" s="13"/>
       <c r="AJ13" s="6">
         <v>1</v>
@@ -1852,25 +1858,25 @@
       <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
       <c r="S14" s="1">
         <v>0</v>
       </c>
@@ -1880,18 +1886,18 @@
       <c r="U14" s="1">
         <v>0</v>
       </c>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="12"/>
-      <c r="AC14" s="12"/>
-      <c r="AD14" s="12"/>
-      <c r="AE14" s="12"/>
-      <c r="AF14" s="12"/>
-      <c r="AG14" s="12"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
+      <c r="AG14" s="14"/>
       <c r="AI14" s="13"/>
       <c r="AJ14" s="6">
         <v>1</v>
@@ -1913,23 +1919,23 @@
       <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
       <c r="S15" s="1">
         <v>0</v>
       </c>
@@ -1939,18 +1945,18 @@
       <c r="U15" s="1">
         <v>1</v>
       </c>
-      <c r="V15" s="12"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="12"/>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="12"/>
-      <c r="AC15" s="12"/>
-      <c r="AD15" s="12"/>
-      <c r="AE15" s="12"/>
-      <c r="AF15" s="12"/>
-      <c r="AG15" s="12"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="14"/>
+      <c r="AE15" s="14"/>
+      <c r="AF15" s="14"/>
+      <c r="AG15" s="14"/>
       <c r="AI15" s="13"/>
       <c r="AJ15" s="6">
         <v>1</v>
@@ -1972,23 +1978,23 @@
       <c r="A16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
       <c r="S16" s="1">
         <v>1</v>
       </c>
@@ -1998,18 +2004,18 @@
       <c r="U16" s="1">
         <v>0</v>
       </c>
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="12"/>
-      <c r="AC16" s="12"/>
-      <c r="AD16" s="12"/>
-      <c r="AE16" s="12"/>
-      <c r="AF16" s="12"/>
-      <c r="AG16" s="12"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="14"/>
+      <c r="AE16" s="14"/>
+      <c r="AF16" s="14"/>
+      <c r="AG16" s="14"/>
       <c r="AI16" s="13"/>
       <c r="AJ16" s="6">
         <v>1</v>
@@ -2049,19 +2055,19 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
       <c r="S17" s="1">
         <v>1</v>
       </c>
@@ -2071,18 +2077,18 @@
       <c r="U17" s="1">
         <v>1</v>
       </c>
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
-      <c r="AB17" s="12"/>
-      <c r="AC17" s="12"/>
-      <c r="AD17" s="12"/>
-      <c r="AE17" s="12"/>
-      <c r="AF17" s="12"/>
-      <c r="AG17" s="12"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="14"/>
+      <c r="X17" s="14"/>
+      <c r="Y17" s="14"/>
+      <c r="Z17" s="14"/>
+      <c r="AA17" s="14"/>
+      <c r="AB17" s="14"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="14"/>
+      <c r="AE17" s="14"/>
+      <c r="AF17" s="14"/>
+      <c r="AG17" s="14"/>
       <c r="AI17" s="13"/>
       <c r="AJ17" s="6">
         <v>1</v>
@@ -2122,17 +2128,17 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
       <c r="S18" s="1">
         <v>1</v>
       </c>
@@ -2142,18 +2148,18 @@
       <c r="U18" s="1">
         <v>1</v>
       </c>
-      <c r="V18" s="12"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="12"/>
-      <c r="Y18" s="12"/>
-      <c r="Z18" s="12"/>
-      <c r="AA18" s="12"/>
-      <c r="AB18" s="12"/>
-      <c r="AC18" s="12"/>
-      <c r="AD18" s="12"/>
-      <c r="AE18" s="12"/>
-      <c r="AF18" s="12"/>
-      <c r="AG18" s="12"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="14"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="14"/>
+      <c r="AG18" s="14"/>
       <c r="AI18" s="13"/>
       <c r="AJ18" s="6">
         <v>1</v>
@@ -2175,25 +2181,25 @@
       <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
       <c r="S19" s="1">
         <v>1</v>
       </c>
@@ -2203,18 +2209,18 @@
       <c r="U19" s="1">
         <v>0</v>
       </c>
-      <c r="V19" s="12"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="12"/>
-      <c r="Z19" s="12"/>
-      <c r="AA19" s="12"/>
-      <c r="AB19" s="12"/>
-      <c r="AC19" s="12"/>
-      <c r="AD19" s="12"/>
-      <c r="AE19" s="12"/>
-      <c r="AF19" s="12"/>
-      <c r="AG19" s="12"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="14"/>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="14"/>
+      <c r="AA19" s="14"/>
+      <c r="AB19" s="14"/>
+      <c r="AC19" s="14"/>
+      <c r="AD19" s="14"/>
+      <c r="AE19" s="14"/>
+      <c r="AF19" s="14"/>
+      <c r="AG19" s="14"/>
       <c r="AI19" s="13"/>
       <c r="AJ19" s="6">
         <v>1</v>
@@ -2236,23 +2242,23 @@
       <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="12"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
       <c r="S20" s="1">
         <v>1</v>
       </c>
@@ -2262,18 +2268,18 @@
       <c r="U20" s="1">
         <v>1</v>
       </c>
-      <c r="V20" s="12"/>
-      <c r="W20" s="12"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="12"/>
-      <c r="Z20" s="12"/>
-      <c r="AA20" s="12"/>
-      <c r="AB20" s="12"/>
-      <c r="AC20" s="12"/>
-      <c r="AD20" s="12"/>
-      <c r="AE20" s="12"/>
-      <c r="AF20" s="12"/>
-      <c r="AG20" s="12"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="14"/>
+      <c r="AB20" s="14"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="14"/>
+      <c r="AE20" s="14"/>
+      <c r="AF20" s="14"/>
+      <c r="AG20" s="14"/>
       <c r="AI20" s="13"/>
       <c r="AJ20" s="6">
         <v>1</v>
@@ -2295,31 +2301,31 @@
       <c r="A21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="14">
         <v>0</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
       </c>
-      <c r="D21" s="12">
-        <v>0</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12" t="s">
+      <c r="D21" s="14">
+        <v>0</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
       <c r="S21" s="1">
         <v>0</v>
       </c>
@@ -2329,30 +2335,30 @@
       <c r="U21" s="1">
         <v>0</v>
       </c>
-      <c r="V21" s="12"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="12"/>
-      <c r="Z21" s="12"/>
-      <c r="AA21" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB21" s="12">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="12">
-        <v>1</v>
-      </c>
-      <c r="AD21" s="12">
-        <v>0</v>
-      </c>
-      <c r="AE21" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF21" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG21" s="12">
+      <c r="V21" s="14"/>
+      <c r="W21" s="14"/>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="14"/>
+      <c r="Z21" s="14"/>
+      <c r="AA21" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="14">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="14">
         <v>1</v>
       </c>
       <c r="AI21" s="13" t="s">
@@ -2378,25 +2384,25 @@
       <c r="A22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="12"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
       <c r="S22" s="1">
         <v>0</v>
       </c>
@@ -2406,18 +2412,18 @@
       <c r="U22" s="1">
         <v>0</v>
       </c>
-      <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
-      <c r="AA22" s="12"/>
-      <c r="AB22" s="12"/>
-      <c r="AC22" s="12"/>
-      <c r="AD22" s="12"/>
-      <c r="AE22" s="12"/>
-      <c r="AF22" s="12"/>
-      <c r="AG22" s="12"/>
+      <c r="V22" s="14"/>
+      <c r="W22" s="14"/>
+      <c r="X22" s="14"/>
+      <c r="Y22" s="14"/>
+      <c r="Z22" s="14"/>
+      <c r="AA22" s="14"/>
+      <c r="AB22" s="14"/>
+      <c r="AC22" s="14"/>
+      <c r="AD22" s="14"/>
+      <c r="AE22" s="14"/>
+      <c r="AF22" s="14"/>
+      <c r="AG22" s="14"/>
       <c r="AI22" s="13"/>
       <c r="AJ22" s="6">
         <v>1</v>
@@ -2439,25 +2445,25 @@
       <c r="A23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="12"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="1">
         <v>0</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
       <c r="S23" s="1">
         <v>0</v>
       </c>
@@ -2467,18 +2473,18 @@
       <c r="U23" s="1">
         <v>1</v>
       </c>
-      <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="12"/>
-      <c r="Z23" s="12"/>
-      <c r="AA23" s="12"/>
-      <c r="AB23" s="12"/>
-      <c r="AC23" s="12"/>
-      <c r="AD23" s="12"/>
-      <c r="AE23" s="12"/>
-      <c r="AF23" s="12"/>
-      <c r="AG23" s="12"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="14"/>
+      <c r="AD23" s="14"/>
+      <c r="AE23" s="14"/>
+      <c r="AF23" s="14"/>
+      <c r="AG23" s="14"/>
       <c r="AI23" s="13"/>
       <c r="AJ23" s="6">
         <v>1</v>
@@ -2500,25 +2506,25 @@
       <c r="A24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="12"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="1">
         <v>0</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
       <c r="S24" s="1">
         <v>0</v>
       </c>
@@ -2528,18 +2534,18 @@
       <c r="U24" s="1">
         <v>0</v>
       </c>
-      <c r="V24" s="12"/>
-      <c r="W24" s="12"/>
-      <c r="X24" s="12"/>
-      <c r="Y24" s="12"/>
-      <c r="Z24" s="12"/>
-      <c r="AA24" s="12"/>
-      <c r="AB24" s="12"/>
-      <c r="AC24" s="12"/>
-      <c r="AD24" s="12"/>
-      <c r="AE24" s="12"/>
-      <c r="AF24" s="12"/>
-      <c r="AG24" s="12"/>
+      <c r="V24" s="14"/>
+      <c r="W24" s="14"/>
+      <c r="X24" s="14"/>
+      <c r="Y24" s="14"/>
+      <c r="Z24" s="14"/>
+      <c r="AA24" s="14"/>
+      <c r="AB24" s="14"/>
+      <c r="AC24" s="14"/>
+      <c r="AD24" s="14"/>
+      <c r="AE24" s="14"/>
+      <c r="AF24" s="14"/>
+      <c r="AG24" s="14"/>
       <c r="AI24" s="13"/>
       <c r="AJ24" s="6">
         <v>1</v>
@@ -2561,25 +2567,25 @@
       <c r="A25" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="1">
         <v>0</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
       <c r="S25" s="1">
         <v>0</v>
       </c>
@@ -2589,18 +2595,18 @@
       <c r="U25" s="1">
         <v>1</v>
       </c>
-      <c r="V25" s="12"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="12"/>
-      <c r="Y25" s="12"/>
-      <c r="Z25" s="12"/>
-      <c r="AA25" s="12"/>
-      <c r="AB25" s="12"/>
-      <c r="AC25" s="12"/>
-      <c r="AD25" s="12"/>
-      <c r="AE25" s="12"/>
-      <c r="AF25" s="12"/>
-      <c r="AG25" s="12"/>
+      <c r="V25" s="14"/>
+      <c r="W25" s="14"/>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="14"/>
+      <c r="Z25" s="14"/>
+      <c r="AA25" s="14"/>
+      <c r="AB25" s="14"/>
+      <c r="AC25" s="14"/>
+      <c r="AD25" s="14"/>
+      <c r="AE25" s="14"/>
+      <c r="AF25" s="14"/>
+      <c r="AG25" s="14"/>
       <c r="AI25" s="13"/>
       <c r="AJ25" s="6">
         <v>1</v>
@@ -2622,25 +2628,25 @@
       <c r="A26" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="1">
         <v>0</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
       <c r="S26" s="1">
         <v>1</v>
       </c>
@@ -2650,18 +2656,18 @@
       <c r="U26" s="1">
         <v>0</v>
       </c>
-      <c r="V26" s="12"/>
-      <c r="W26" s="12"/>
-      <c r="X26" s="12"/>
-      <c r="Y26" s="12"/>
-      <c r="Z26" s="12"/>
-      <c r="AA26" s="12"/>
-      <c r="AB26" s="12"/>
-      <c r="AC26" s="12"/>
-      <c r="AD26" s="12"/>
-      <c r="AE26" s="12"/>
-      <c r="AF26" s="12"/>
-      <c r="AG26" s="12"/>
+      <c r="V26" s="14"/>
+      <c r="W26" s="14"/>
+      <c r="X26" s="14"/>
+      <c r="Y26" s="14"/>
+      <c r="Z26" s="14"/>
+      <c r="AA26" s="14"/>
+      <c r="AB26" s="14"/>
+      <c r="AC26" s="14"/>
+      <c r="AD26" s="14"/>
+      <c r="AE26" s="14"/>
+      <c r="AF26" s="14"/>
+      <c r="AG26" s="14"/>
       <c r="AI26" s="13"/>
       <c r="AJ26" s="6">
         <v>1</v>
@@ -2683,25 +2689,25 @@
       <c r="A27" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="1">
         <v>0</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
       <c r="S27" s="1">
         <v>1</v>
       </c>
@@ -2711,18 +2717,18 @@
       <c r="U27" s="1">
         <v>1</v>
       </c>
-      <c r="V27" s="12"/>
-      <c r="W27" s="12"/>
-      <c r="X27" s="12"/>
-      <c r="Y27" s="12"/>
-      <c r="Z27" s="12"/>
-      <c r="AA27" s="12"/>
-      <c r="AB27" s="12"/>
-      <c r="AC27" s="12"/>
-      <c r="AD27" s="12"/>
-      <c r="AE27" s="12"/>
-      <c r="AF27" s="12"/>
-      <c r="AG27" s="12"/>
+      <c r="V27" s="14"/>
+      <c r="W27" s="14"/>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="14"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="14"/>
+      <c r="AB27" s="14"/>
+      <c r="AC27" s="14"/>
+      <c r="AD27" s="14"/>
+      <c r="AE27" s="14"/>
+      <c r="AF27" s="14"/>
+      <c r="AG27" s="14"/>
       <c r="AI27" s="13"/>
       <c r="AJ27" s="6">
         <v>1</v>
@@ -2744,25 +2750,25 @@
       <c r="A28" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
       <c r="S28" s="1">
         <v>1</v>
       </c>
@@ -2772,18 +2778,18 @@
       <c r="U28" s="1">
         <v>1</v>
       </c>
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
-      <c r="X28" s="12"/>
-      <c r="Y28" s="12"/>
-      <c r="Z28" s="12"/>
-      <c r="AA28" s="12"/>
-      <c r="AB28" s="12"/>
-      <c r="AC28" s="12"/>
-      <c r="AD28" s="12"/>
-      <c r="AE28" s="12"/>
-      <c r="AF28" s="12"/>
-      <c r="AG28" s="12"/>
+      <c r="V28" s="14"/>
+      <c r="W28" s="14"/>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="14"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="14"/>
+      <c r="AB28" s="14"/>
+      <c r="AC28" s="14"/>
+      <c r="AD28" s="14"/>
+      <c r="AE28" s="14"/>
+      <c r="AF28" s="14"/>
+      <c r="AG28" s="14"/>
       <c r="AI28" s="13"/>
       <c r="AJ28" s="6">
         <v>1</v>
@@ -2805,25 +2811,25 @@
       <c r="A29" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="12"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="1">
         <v>0</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="12"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
       <c r="S29" s="1">
         <v>1</v>
       </c>
@@ -2833,18 +2839,18 @@
       <c r="U29" s="1">
         <v>0</v>
       </c>
-      <c r="V29" s="12"/>
-      <c r="W29" s="12"/>
-      <c r="X29" s="12"/>
-      <c r="Y29" s="12"/>
-      <c r="Z29" s="12"/>
-      <c r="AA29" s="12"/>
-      <c r="AB29" s="12"/>
-      <c r="AC29" s="12"/>
-      <c r="AD29" s="12"/>
-      <c r="AE29" s="12"/>
-      <c r="AF29" s="12"/>
-      <c r="AG29" s="12"/>
+      <c r="V29" s="14"/>
+      <c r="W29" s="14"/>
+      <c r="X29" s="14"/>
+      <c r="Y29" s="14"/>
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="14"/>
+      <c r="AB29" s="14"/>
+      <c r="AC29" s="14"/>
+      <c r="AD29" s="14"/>
+      <c r="AE29" s="14"/>
+      <c r="AF29" s="14"/>
+      <c r="AG29" s="14"/>
       <c r="AI29" s="13"/>
       <c r="AJ29" s="6">
         <v>1</v>
@@ -2866,25 +2872,25 @@
       <c r="A30" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="1">
         <v>0</v>
       </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="12"/>
-      <c r="R30" s="12"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
       <c r="S30" s="1">
         <v>1</v>
       </c>
@@ -2894,18 +2900,18 @@
       <c r="U30" s="1">
         <v>1</v>
       </c>
-      <c r="V30" s="12"/>
-      <c r="W30" s="12"/>
-      <c r="X30" s="12"/>
-      <c r="Y30" s="12"/>
-      <c r="Z30" s="12"/>
-      <c r="AA30" s="12"/>
-      <c r="AB30" s="12"/>
-      <c r="AC30" s="12"/>
-      <c r="AD30" s="12"/>
-      <c r="AE30" s="12"/>
-      <c r="AF30" s="12"/>
-      <c r="AG30" s="12"/>
+      <c r="V30" s="14"/>
+      <c r="W30" s="14"/>
+      <c r="X30" s="14"/>
+      <c r="Y30" s="14"/>
+      <c r="Z30" s="14"/>
+      <c r="AA30" s="14"/>
+      <c r="AB30" s="14"/>
+      <c r="AC30" s="14"/>
+      <c r="AD30" s="14"/>
+      <c r="AE30" s="14"/>
+      <c r="AF30" s="14"/>
+      <c r="AG30" s="14"/>
       <c r="AI30" s="13"/>
       <c r="AJ30" s="6">
         <v>1</v>
@@ -2927,25 +2933,25 @@
       <c r="A31" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
       <c r="S31" s="1">
         <v>0</v>
       </c>
@@ -2955,30 +2961,30 @@
       <c r="U31" s="1">
         <v>0</v>
       </c>
-      <c r="V31" s="12"/>
-      <c r="W31" s="12"/>
-      <c r="X31" s="12"/>
-      <c r="Y31" s="12"/>
-      <c r="Z31" s="12"/>
-      <c r="AA31" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB31" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="12">
-        <v>1</v>
-      </c>
-      <c r="AD31" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE31" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF31" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG31" s="12">
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+      <c r="Z31" s="14"/>
+      <c r="AA31" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="14">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="14">
+        <v>1</v>
+      </c>
+      <c r="AE31" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="14">
         <v>1</v>
       </c>
       <c r="AI31" s="13" t="s">
@@ -2995,25 +3001,25 @@
       <c r="C32" s="1">
         <v>0</v>
       </c>
-      <c r="D32" s="12">
-        <v>0</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12" t="s">
+      <c r="D32" s="14">
+        <v>0</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="12"/>
-      <c r="R32" s="12"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
       <c r="S32" s="1">
         <v>0</v>
       </c>
@@ -3023,18 +3029,18 @@
       <c r="U32" s="1">
         <v>1</v>
       </c>
-      <c r="V32" s="12"/>
-      <c r="W32" s="12"/>
-      <c r="X32" s="12"/>
-      <c r="Y32" s="12"/>
-      <c r="Z32" s="12"/>
-      <c r="AA32" s="12"/>
-      <c r="AB32" s="12"/>
-      <c r="AC32" s="12"/>
-      <c r="AD32" s="12"/>
-      <c r="AE32" s="12"/>
-      <c r="AF32" s="12"/>
-      <c r="AG32" s="12"/>
+      <c r="V32" s="14"/>
+      <c r="W32" s="14"/>
+      <c r="X32" s="14"/>
+      <c r="Y32" s="14"/>
+      <c r="Z32" s="14"/>
+      <c r="AA32" s="14"/>
+      <c r="AB32" s="14"/>
+      <c r="AC32" s="14"/>
+      <c r="AD32" s="14"/>
+      <c r="AE32" s="14"/>
+      <c r="AF32" s="14"/>
+      <c r="AG32" s="14"/>
       <c r="AI32" s="13"/>
     </row>
     <row r="33" spans="1:48" x14ac:dyDescent="0.3">
@@ -3047,21 +3053,21 @@
       <c r="C33" s="1">
         <v>0</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="12"/>
-      <c r="R33" s="12"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
       <c r="S33" s="1">
         <v>1</v>
       </c>
@@ -3071,18 +3077,18 @@
       <c r="U33" s="1">
         <v>1</v>
       </c>
-      <c r="V33" s="12"/>
-      <c r="W33" s="12"/>
-      <c r="X33" s="12"/>
-      <c r="Y33" s="12"/>
-      <c r="Z33" s="12"/>
-      <c r="AA33" s="12"/>
-      <c r="AB33" s="12"/>
-      <c r="AC33" s="12"/>
-      <c r="AD33" s="12"/>
-      <c r="AE33" s="12"/>
-      <c r="AF33" s="12"/>
-      <c r="AG33" s="12"/>
+      <c r="V33" s="14"/>
+      <c r="W33" s="14"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="14"/>
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="14"/>
+      <c r="AB33" s="14"/>
+      <c r="AC33" s="14"/>
+      <c r="AD33" s="14"/>
+      <c r="AE33" s="14"/>
+      <c r="AF33" s="14"/>
+      <c r="AG33" s="14"/>
       <c r="AI33" s="13"/>
     </row>
     <row r="34" spans="1:48" x14ac:dyDescent="0.3">
@@ -3095,21 +3101,21 @@
       <c r="C34" s="1">
         <v>1</v>
       </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="12"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
       <c r="S34" s="1">
         <v>1</v>
       </c>
@@ -3119,18 +3125,18 @@
       <c r="U34" s="1">
         <v>1</v>
       </c>
-      <c r="V34" s="12"/>
-      <c r="W34" s="12"/>
-      <c r="X34" s="12"/>
-      <c r="Y34" s="12"/>
-      <c r="Z34" s="12"/>
-      <c r="AA34" s="12"/>
-      <c r="AB34" s="12"/>
-      <c r="AC34" s="12"/>
-      <c r="AD34" s="12"/>
-      <c r="AE34" s="12"/>
-      <c r="AF34" s="12"/>
-      <c r="AG34" s="12"/>
+      <c r="V34" s="14"/>
+      <c r="W34" s="14"/>
+      <c r="X34" s="14"/>
+      <c r="Y34" s="14"/>
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="14"/>
+      <c r="AB34" s="14"/>
+      <c r="AC34" s="14"/>
+      <c r="AD34" s="14"/>
+      <c r="AE34" s="14"/>
+      <c r="AF34" s="14"/>
+      <c r="AG34" s="14"/>
       <c r="AI34" s="13"/>
     </row>
     <row r="35" spans="1:48" x14ac:dyDescent="0.3">
@@ -3143,23 +3149,23 @@
       <c r="C35" s="1">
         <v>0</v>
       </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12" t="s">
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="12"/>
-      <c r="R35" s="12"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
       <c r="S35" s="1">
         <v>0</v>
       </c>
@@ -3169,30 +3175,30 @@
       <c r="U35" s="1">
         <v>0</v>
       </c>
-      <c r="V35" s="12"/>
-      <c r="W35" s="12"/>
-      <c r="X35" s="12"/>
-      <c r="Y35" s="12"/>
-      <c r="Z35" s="12"/>
-      <c r="AA35" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB35" s="12">
-        <v>1</v>
-      </c>
-      <c r="AC35" s="12">
-        <v>1</v>
-      </c>
-      <c r="AD35" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE35" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF35" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG35" s="12">
+      <c r="V35" s="14"/>
+      <c r="W35" s="14"/>
+      <c r="X35" s="14"/>
+      <c r="Y35" s="14"/>
+      <c r="Z35" s="14"/>
+      <c r="AA35" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="14">
+        <v>1</v>
+      </c>
+      <c r="AD35" s="14">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="14">
         <v>1</v>
       </c>
       <c r="AI35" s="13" t="s">
@@ -3209,21 +3215,21 @@
       <c r="C36" s="1">
         <v>1</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
-      <c r="R36" s="12"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
       <c r="S36" s="1">
         <v>0</v>
       </c>
@@ -3233,18 +3239,18 @@
       <c r="U36" s="1">
         <v>0</v>
       </c>
-      <c r="V36" s="12"/>
-      <c r="W36" s="12"/>
-      <c r="X36" s="12"/>
-      <c r="Y36" s="12"/>
-      <c r="Z36" s="12"/>
-      <c r="AA36" s="12"/>
-      <c r="AB36" s="12"/>
-      <c r="AC36" s="12"/>
-      <c r="AD36" s="12"/>
-      <c r="AE36" s="12"/>
-      <c r="AF36" s="12"/>
-      <c r="AG36" s="12"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="14"/>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="14"/>
+      <c r="Z36" s="14"/>
+      <c r="AA36" s="14"/>
+      <c r="AB36" s="14"/>
+      <c r="AC36" s="14"/>
+      <c r="AD36" s="14"/>
+      <c r="AE36" s="14"/>
+      <c r="AF36" s="14"/>
+      <c r="AG36" s="14"/>
       <c r="AI36" s="13"/>
     </row>
     <row r="37" spans="1:48" x14ac:dyDescent="0.3">
@@ -3257,21 +3263,21 @@
       <c r="C37" s="1">
         <v>0</v>
       </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="12"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
       <c r="S37" s="1">
         <v>0</v>
       </c>
@@ -3281,18 +3287,18 @@
       <c r="U37" s="1">
         <v>1</v>
       </c>
-      <c r="V37" s="12"/>
-      <c r="W37" s="12"/>
-      <c r="X37" s="12"/>
-      <c r="Y37" s="12"/>
-      <c r="Z37" s="12"/>
-      <c r="AA37" s="12"/>
-      <c r="AB37" s="12"/>
-      <c r="AC37" s="12"/>
-      <c r="AD37" s="12"/>
-      <c r="AE37" s="12"/>
-      <c r="AF37" s="12"/>
-      <c r="AG37" s="12"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="14"/>
+      <c r="AF37" s="14"/>
+      <c r="AG37" s="14"/>
       <c r="AI37" s="13"/>
     </row>
     <row r="38" spans="1:48" x14ac:dyDescent="0.3">
@@ -3305,21 +3311,21 @@
       <c r="C38" s="1">
         <v>0</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="12"/>
-      <c r="Q38" s="12"/>
-      <c r="R38" s="12"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
       <c r="S38" s="1">
         <v>1</v>
       </c>
@@ -3329,18 +3335,18 @@
       <c r="U38" s="1">
         <v>1</v>
       </c>
-      <c r="V38" s="12"/>
-      <c r="W38" s="12"/>
-      <c r="X38" s="12"/>
-      <c r="Y38" s="12"/>
-      <c r="Z38" s="12"/>
-      <c r="AA38" s="12"/>
-      <c r="AB38" s="12"/>
-      <c r="AC38" s="12"/>
-      <c r="AD38" s="12"/>
-      <c r="AE38" s="12"/>
-      <c r="AF38" s="12"/>
-      <c r="AG38" s="12"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="14"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="14"/>
+      <c r="Z38" s="14"/>
+      <c r="AA38" s="14"/>
+      <c r="AB38" s="14"/>
+      <c r="AC38" s="14"/>
+      <c r="AD38" s="14"/>
+      <c r="AE38" s="14"/>
+      <c r="AF38" s="14"/>
+      <c r="AG38" s="14"/>
       <c r="AI38" s="13"/>
     </row>
     <row r="39" spans="1:48" x14ac:dyDescent="0.3">
@@ -3353,21 +3359,21 @@
       <c r="C39" s="1">
         <v>1</v>
       </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
-      <c r="P39" s="12"/>
-      <c r="Q39" s="12"/>
-      <c r="R39" s="12"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
       <c r="S39" s="1">
         <v>1</v>
       </c>
@@ -3377,43 +3383,43 @@
       <c r="U39" s="1">
         <v>1</v>
       </c>
-      <c r="V39" s="12"/>
-      <c r="W39" s="12"/>
-      <c r="X39" s="12"/>
-      <c r="Y39" s="12"/>
-      <c r="Z39" s="12"/>
-      <c r="AA39" s="12"/>
-      <c r="AB39" s="12"/>
-      <c r="AC39" s="12"/>
-      <c r="AD39" s="12"/>
-      <c r="AE39" s="12"/>
-      <c r="AF39" s="12"/>
-      <c r="AG39" s="12"/>
+      <c r="V39" s="14"/>
+      <c r="W39" s="14"/>
+      <c r="X39" s="14"/>
+      <c r="Y39" s="14"/>
+      <c r="Z39" s="14"/>
+      <c r="AA39" s="14"/>
+      <c r="AB39" s="14"/>
+      <c r="AC39" s="14"/>
+      <c r="AD39" s="14"/>
+      <c r="AE39" s="14"/>
+      <c r="AF39" s="14"/>
+      <c r="AG39" s="14"/>
       <c r="AI39" s="13"/>
     </row>
     <row r="40" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
-      <c r="O40" s="12"/>
-      <c r="P40" s="12"/>
-      <c r="Q40" s="12"/>
-      <c r="R40" s="12"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
       <c r="S40" s="1">
         <v>0</v>
       </c>
@@ -3423,30 +3429,30 @@
       <c r="U40" s="1">
         <v>0</v>
       </c>
-      <c r="V40" s="12"/>
-      <c r="W40" s="12"/>
-      <c r="X40" s="12"/>
-      <c r="Y40" s="12"/>
-      <c r="Z40" s="12"/>
-      <c r="AA40" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD40" s="12">
-        <v>0</v>
-      </c>
-      <c r="AE40" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF40" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG40" s="12">
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14"/>
+      <c r="Z40" s="14"/>
+      <c r="AA40" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF40" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG40" s="14">
         <v>1</v>
       </c>
       <c r="AI40" s="13" t="s">
@@ -3478,23 +3484,23 @@
       <c r="A41" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="12"/>
-      <c r="Q41" s="12"/>
-      <c r="R41" s="12"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
       <c r="S41" s="1">
         <v>0</v>
       </c>
@@ -3504,18 +3510,18 @@
       <c r="U41" s="1">
         <v>1</v>
       </c>
-      <c r="V41" s="12"/>
-      <c r="W41" s="12"/>
-      <c r="X41" s="12"/>
-      <c r="Y41" s="12"/>
-      <c r="Z41" s="12"/>
-      <c r="AA41" s="12"/>
-      <c r="AB41" s="12"/>
-      <c r="AC41" s="12"/>
-      <c r="AD41" s="12"/>
-      <c r="AE41" s="12"/>
-      <c r="AF41" s="12"/>
-      <c r="AG41" s="12"/>
+      <c r="V41" s="14"/>
+      <c r="W41" s="14"/>
+      <c r="X41" s="14"/>
+      <c r="Y41" s="14"/>
+      <c r="Z41" s="14"/>
+      <c r="AA41" s="14"/>
+      <c r="AB41" s="14"/>
+      <c r="AC41" s="14"/>
+      <c r="AD41" s="14"/>
+      <c r="AE41" s="14"/>
+      <c r="AF41" s="14"/>
+      <c r="AG41" s="14"/>
       <c r="AI41" s="13"/>
       <c r="AJ41" s="6">
         <v>1</v>
@@ -3543,23 +3549,23 @@
       <c r="A42" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
-      <c r="O42" s="12"/>
-      <c r="P42" s="12"/>
-      <c r="Q42" s="12"/>
-      <c r="R42" s="12"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
       <c r="S42" s="1">
         <v>0</v>
       </c>
@@ -3569,18 +3575,18 @@
       <c r="U42" s="1">
         <v>0</v>
       </c>
-      <c r="V42" s="12"/>
-      <c r="W42" s="12"/>
-      <c r="X42" s="12"/>
-      <c r="Y42" s="12"/>
-      <c r="Z42" s="12"/>
-      <c r="AA42" s="12"/>
-      <c r="AB42" s="12"/>
-      <c r="AC42" s="12"/>
-      <c r="AD42" s="12"/>
-      <c r="AE42" s="12"/>
-      <c r="AF42" s="12"/>
-      <c r="AG42" s="12"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
+      <c r="Z42" s="14"/>
+      <c r="AA42" s="14"/>
+      <c r="AB42" s="14"/>
+      <c r="AC42" s="14"/>
+      <c r="AD42" s="14"/>
+      <c r="AE42" s="14"/>
+      <c r="AF42" s="14"/>
+      <c r="AG42" s="14"/>
       <c r="AI42" s="13"/>
       <c r="AJ42" s="6">
         <v>1</v>
@@ -3608,23 +3614,23 @@
       <c r="A43" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
-      <c r="P43" s="12"/>
-      <c r="Q43" s="12"/>
-      <c r="R43" s="12"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
       <c r="S43" s="1">
         <v>0</v>
       </c>
@@ -3634,18 +3640,18 @@
       <c r="U43" s="1">
         <v>1</v>
       </c>
-      <c r="V43" s="12"/>
-      <c r="W43" s="12"/>
-      <c r="X43" s="12"/>
-      <c r="Y43" s="12"/>
-      <c r="Z43" s="12"/>
-      <c r="AA43" s="12"/>
-      <c r="AB43" s="12"/>
-      <c r="AC43" s="12"/>
-      <c r="AD43" s="12"/>
-      <c r="AE43" s="12"/>
-      <c r="AF43" s="12"/>
-      <c r="AG43" s="12"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+      <c r="Z43" s="14"/>
+      <c r="AA43" s="14"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="14"/>
+      <c r="AD43" s="14"/>
+      <c r="AE43" s="14"/>
+      <c r="AF43" s="14"/>
+      <c r="AG43" s="14"/>
       <c r="AI43" s="13"/>
       <c r="AN43" s="10"/>
       <c r="AO43" s="10"/>
@@ -3655,23 +3661,23 @@
       <c r="A44" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
-      <c r="P44" s="12"/>
-      <c r="Q44" s="12"/>
-      <c r="R44" s="12"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
       <c r="S44" s="1">
         <v>1</v>
       </c>
@@ -3681,18 +3687,18 @@
       <c r="U44" s="1">
         <v>0</v>
       </c>
-      <c r="V44" s="12"/>
-      <c r="W44" s="12"/>
-      <c r="X44" s="12"/>
-      <c r="Y44" s="12"/>
-      <c r="Z44" s="12"/>
-      <c r="AA44" s="12"/>
-      <c r="AB44" s="12"/>
-      <c r="AC44" s="12"/>
-      <c r="AD44" s="12"/>
-      <c r="AE44" s="12"/>
-      <c r="AF44" s="12"/>
-      <c r="AG44" s="12"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="14"/>
+      <c r="X44" s="14"/>
+      <c r="Y44" s="14"/>
+      <c r="Z44" s="14"/>
+      <c r="AA44" s="14"/>
+      <c r="AB44" s="14"/>
+      <c r="AC44" s="14"/>
+      <c r="AD44" s="14"/>
+      <c r="AE44" s="14"/>
+      <c r="AF44" s="14"/>
+      <c r="AG44" s="14"/>
       <c r="AI44" s="13"/>
       <c r="AJ44" s="6">
         <v>1</v>
@@ -3720,23 +3726,23 @@
       <c r="A45" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
-      <c r="P45" s="12"/>
-      <c r="Q45" s="12"/>
-      <c r="R45" s="12"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
       <c r="S45" s="1">
         <v>1</v>
       </c>
@@ -3746,18 +3752,18 @@
       <c r="U45" s="1">
         <v>1</v>
       </c>
-      <c r="V45" s="12"/>
-      <c r="W45" s="12"/>
-      <c r="X45" s="12"/>
-      <c r="Y45" s="12"/>
-      <c r="Z45" s="12"/>
-      <c r="AA45" s="12"/>
-      <c r="AB45" s="12"/>
-      <c r="AC45" s="12"/>
-      <c r="AD45" s="12"/>
-      <c r="AE45" s="12"/>
-      <c r="AF45" s="12"/>
-      <c r="AG45" s="12"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="14"/>
+      <c r="X45" s="14"/>
+      <c r="Y45" s="14"/>
+      <c r="Z45" s="14"/>
+      <c r="AA45" s="14"/>
+      <c r="AB45" s="14"/>
+      <c r="AC45" s="14"/>
+      <c r="AD45" s="14"/>
+      <c r="AE45" s="14"/>
+      <c r="AF45" s="14"/>
+      <c r="AG45" s="14"/>
       <c r="AI45" s="13"/>
       <c r="AJ45" s="6">
         <v>1</v>
@@ -3785,23 +3791,23 @@
       <c r="A46" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-      <c r="O46" s="12"/>
-      <c r="P46" s="12"/>
-      <c r="Q46" s="12"/>
-      <c r="R46" s="12"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
       <c r="S46" s="1">
         <v>1</v>
       </c>
@@ -3811,18 +3817,18 @@
       <c r="U46" s="1">
         <v>0</v>
       </c>
-      <c r="V46" s="12"/>
-      <c r="W46" s="12"/>
-      <c r="X46" s="12"/>
-      <c r="Y46" s="12"/>
-      <c r="Z46" s="12"/>
-      <c r="AA46" s="12"/>
-      <c r="AB46" s="12"/>
-      <c r="AC46" s="12"/>
-      <c r="AD46" s="12"/>
-      <c r="AE46" s="12"/>
-      <c r="AF46" s="12"/>
-      <c r="AG46" s="12"/>
+      <c r="V46" s="14"/>
+      <c r="W46" s="14"/>
+      <c r="X46" s="14"/>
+      <c r="Y46" s="14"/>
+      <c r="Z46" s="14"/>
+      <c r="AA46" s="14"/>
+      <c r="AB46" s="14"/>
+      <c r="AC46" s="14"/>
+      <c r="AD46" s="14"/>
+      <c r="AE46" s="14"/>
+      <c r="AF46" s="14"/>
+      <c r="AG46" s="14"/>
       <c r="AI46" s="13"/>
       <c r="AJ46" s="6">
         <v>1</v>
@@ -3847,27 +3853,27 @@
       <c r="A47" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12" t="s">
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J47" s="12"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-      <c r="O47" s="12"/>
-      <c r="P47" s="12"/>
-      <c r="Q47" s="12"/>
-      <c r="R47" s="12"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
       <c r="S47" s="1">
         <v>0</v>
       </c>
@@ -3877,32 +3883,32 @@
       <c r="U47" s="1">
         <v>0</v>
       </c>
-      <c r="V47" s="12" t="s">
+      <c r="V47" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="W47" s="12"/>
-      <c r="X47" s="12"/>
-      <c r="Y47" s="12"/>
-      <c r="Z47" s="12"/>
-      <c r="AA47" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB47" s="12">
-        <v>1</v>
-      </c>
-      <c r="AC47" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD47" s="12">
-        <v>0</v>
-      </c>
-      <c r="AE47" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF47" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG47" s="12">
+      <c r="W47" s="14"/>
+      <c r="X47" s="14"/>
+      <c r="Y47" s="14"/>
+      <c r="Z47" s="14"/>
+      <c r="AA47" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC47" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF47" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="14">
         <v>1</v>
       </c>
       <c r="AI47" s="13" t="s">
@@ -3924,30 +3930,30 @@
         <v>96</v>
       </c>
       <c r="AV47" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
-      <c r="O48" s="12"/>
-      <c r="P48" s="12"/>
-      <c r="Q48" s="12"/>
-      <c r="R48" s="12"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
       <c r="S48" s="1">
         <v>0</v>
       </c>
@@ -3957,18 +3963,18 @@
       <c r="U48" s="1">
         <v>1</v>
       </c>
-      <c r="V48" s="12"/>
-      <c r="W48" s="12"/>
-      <c r="X48" s="12"/>
-      <c r="Y48" s="12"/>
-      <c r="Z48" s="12"/>
-      <c r="AA48" s="12"/>
-      <c r="AB48" s="12"/>
-      <c r="AC48" s="12"/>
-      <c r="AD48" s="12"/>
-      <c r="AE48" s="12"/>
-      <c r="AF48" s="12"/>
-      <c r="AG48" s="12"/>
+      <c r="V48" s="14"/>
+      <c r="W48" s="14"/>
+      <c r="X48" s="14"/>
+      <c r="Y48" s="14"/>
+      <c r="Z48" s="14"/>
+      <c r="AA48" s="14"/>
+      <c r="AB48" s="14"/>
+      <c r="AC48" s="14"/>
+      <c r="AD48" s="14"/>
+      <c r="AE48" s="14"/>
+      <c r="AF48" s="14"/>
+      <c r="AG48" s="14"/>
       <c r="AI48" s="13"/>
       <c r="AK48" s="6">
         <v>1</v>
@@ -3985,31 +3991,31 @@
       <c r="AR48" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="AV48" s="8" t="s">
-        <v>136</v>
+      <c r="AV48" s="12" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-      <c r="K49" s="12"/>
-      <c r="L49" s="12"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-      <c r="O49" s="12"/>
-      <c r="P49" s="12"/>
-      <c r="Q49" s="12"/>
-      <c r="R49" s="12"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="14"/>
       <c r="S49" s="1">
         <v>0</v>
       </c>
@@ -4019,18 +4025,18 @@
       <c r="U49" s="1">
         <v>0</v>
       </c>
-      <c r="V49" s="12"/>
-      <c r="W49" s="12"/>
-      <c r="X49" s="12"/>
-      <c r="Y49" s="12"/>
-      <c r="Z49" s="12"/>
-      <c r="AA49" s="12"/>
-      <c r="AB49" s="12"/>
-      <c r="AC49" s="12"/>
-      <c r="AD49" s="12"/>
-      <c r="AE49" s="12"/>
-      <c r="AF49" s="12"/>
-      <c r="AG49" s="12"/>
+      <c r="V49" s="14"/>
+      <c r="W49" s="14"/>
+      <c r="X49" s="14"/>
+      <c r="Y49" s="14"/>
+      <c r="Z49" s="14"/>
+      <c r="AA49" s="14"/>
+      <c r="AB49" s="14"/>
+      <c r="AC49" s="14"/>
+      <c r="AD49" s="14"/>
+      <c r="AE49" s="14"/>
+      <c r="AF49" s="14"/>
+      <c r="AG49" s="14"/>
       <c r="AI49" s="13"/>
       <c r="AK49" s="6">
         <v>1</v>
@@ -4047,31 +4053,31 @@
       <c r="AR49" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="AV49" s="8" t="s">
-        <v>135</v>
+      <c r="AV49" s="12" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-      <c r="O50" s="12"/>
-      <c r="P50" s="12"/>
-      <c r="Q50" s="12"/>
-      <c r="R50" s="12"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="14"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="14"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="14"/>
+      <c r="R50" s="14"/>
       <c r="S50" s="1">
         <v>0</v>
       </c>
@@ -4081,18 +4087,18 @@
       <c r="U50" s="1">
         <v>1</v>
       </c>
-      <c r="V50" s="12"/>
-      <c r="W50" s="12"/>
-      <c r="X50" s="12"/>
-      <c r="Y50" s="12"/>
-      <c r="Z50" s="12"/>
-      <c r="AA50" s="12"/>
-      <c r="AB50" s="12"/>
-      <c r="AC50" s="12"/>
-      <c r="AD50" s="12"/>
-      <c r="AE50" s="12"/>
-      <c r="AF50" s="12"/>
-      <c r="AG50" s="12"/>
+      <c r="V50" s="14"/>
+      <c r="W50" s="14"/>
+      <c r="X50" s="14"/>
+      <c r="Y50" s="14"/>
+      <c r="Z50" s="14"/>
+      <c r="AA50" s="14"/>
+      <c r="AB50" s="14"/>
+      <c r="AC50" s="14"/>
+      <c r="AD50" s="14"/>
+      <c r="AE50" s="14"/>
+      <c r="AF50" s="14"/>
+      <c r="AG50" s="14"/>
       <c r="AI50" s="13"/>
       <c r="AN50" s="10"/>
       <c r="AO50" s="10"/>
@@ -4100,56 +4106,25 @@
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="AI35:AI39"/>
-    <mergeCell ref="AI40:AI46"/>
-    <mergeCell ref="AI47:AI50"/>
-    <mergeCell ref="AI2:AI7"/>
-    <mergeCell ref="AI10:AI11"/>
-    <mergeCell ref="AI12:AI20"/>
-    <mergeCell ref="AI21:AI30"/>
-    <mergeCell ref="AI31:AI34"/>
-    <mergeCell ref="AG21:AG30"/>
-    <mergeCell ref="D21:H30"/>
-    <mergeCell ref="B21:B30"/>
-    <mergeCell ref="I21:M30"/>
-    <mergeCell ref="AA21:AA30"/>
-    <mergeCell ref="AB21:AB30"/>
-    <mergeCell ref="AC21:AC30"/>
-    <mergeCell ref="AD21:AD30"/>
-    <mergeCell ref="AE21:AE30"/>
-    <mergeCell ref="AF21:AF30"/>
-    <mergeCell ref="AG31:AG34"/>
-    <mergeCell ref="B31:M31"/>
-    <mergeCell ref="AA31:AA34"/>
-    <mergeCell ref="AB31:AB34"/>
-    <mergeCell ref="AC31:AC34"/>
-    <mergeCell ref="AD31:AD34"/>
-    <mergeCell ref="AE31:AE34"/>
-    <mergeCell ref="AF31:AF34"/>
-    <mergeCell ref="AF12:AF20"/>
-    <mergeCell ref="AE2:AE7"/>
-    <mergeCell ref="AF2:AF7"/>
-    <mergeCell ref="AG2:AG7"/>
-    <mergeCell ref="AG12:AG20"/>
-    <mergeCell ref="AB12:AB20"/>
-    <mergeCell ref="AC12:AC20"/>
-    <mergeCell ref="AD12:AD20"/>
-    <mergeCell ref="AE12:AE20"/>
-    <mergeCell ref="B12:M12"/>
-    <mergeCell ref="B14:M16"/>
-    <mergeCell ref="B19:M20"/>
-    <mergeCell ref="H17:M18"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="B2:H7"/>
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="AC2:AC7"/>
-    <mergeCell ref="AD2:AD7"/>
-    <mergeCell ref="AA2:AA7"/>
-    <mergeCell ref="AB2:AB7"/>
-    <mergeCell ref="V2:Z7"/>
-    <mergeCell ref="N2:R7"/>
-    <mergeCell ref="I2:M7"/>
+    <mergeCell ref="AG47:AG50"/>
+    <mergeCell ref="AB47:AB50"/>
+    <mergeCell ref="AC47:AC50"/>
+    <mergeCell ref="AD47:AD50"/>
+    <mergeCell ref="AE47:AE50"/>
+    <mergeCell ref="AF47:AF50"/>
+    <mergeCell ref="B47:H50"/>
+    <mergeCell ref="I47:M50"/>
+    <mergeCell ref="N12:R50"/>
+    <mergeCell ref="V47:Z50"/>
+    <mergeCell ref="AA47:AA50"/>
+    <mergeCell ref="B40:M46"/>
+    <mergeCell ref="V8:Z46"/>
+    <mergeCell ref="I32:M34"/>
+    <mergeCell ref="D32:H39"/>
+    <mergeCell ref="I35:M39"/>
+    <mergeCell ref="B9:U9"/>
+    <mergeCell ref="B10:U11"/>
+    <mergeCell ref="AA12:AA20"/>
     <mergeCell ref="AF35:AF39"/>
     <mergeCell ref="AG35:AG39"/>
     <mergeCell ref="AA40:AA46"/>
@@ -4164,25 +4139,56 @@
     <mergeCell ref="AC35:AC39"/>
     <mergeCell ref="AD35:AD39"/>
     <mergeCell ref="AE35:AE39"/>
-    <mergeCell ref="B47:H50"/>
-    <mergeCell ref="I47:M50"/>
-    <mergeCell ref="N12:R50"/>
-    <mergeCell ref="V47:Z50"/>
-    <mergeCell ref="AA47:AA50"/>
-    <mergeCell ref="B40:M46"/>
-    <mergeCell ref="V8:Z46"/>
-    <mergeCell ref="I32:M34"/>
-    <mergeCell ref="D32:H39"/>
-    <mergeCell ref="I35:M39"/>
-    <mergeCell ref="B9:U9"/>
-    <mergeCell ref="B10:U11"/>
-    <mergeCell ref="AA12:AA20"/>
-    <mergeCell ref="AG47:AG50"/>
-    <mergeCell ref="AB47:AB50"/>
-    <mergeCell ref="AC47:AC50"/>
-    <mergeCell ref="AD47:AD50"/>
-    <mergeCell ref="AE47:AE50"/>
-    <mergeCell ref="AF47:AF50"/>
+    <mergeCell ref="B2:H7"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="AC2:AC7"/>
+    <mergeCell ref="AD2:AD7"/>
+    <mergeCell ref="AA2:AA7"/>
+    <mergeCell ref="AB2:AB7"/>
+    <mergeCell ref="V2:Z7"/>
+    <mergeCell ref="N2:R7"/>
+    <mergeCell ref="I2:M7"/>
+    <mergeCell ref="AB12:AB20"/>
+    <mergeCell ref="AC12:AC20"/>
+    <mergeCell ref="AD12:AD20"/>
+    <mergeCell ref="AE12:AE20"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="B14:M16"/>
+    <mergeCell ref="B19:M20"/>
+    <mergeCell ref="H17:M18"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="AF12:AF20"/>
+    <mergeCell ref="AE2:AE7"/>
+    <mergeCell ref="AF2:AF7"/>
+    <mergeCell ref="AG2:AG7"/>
+    <mergeCell ref="AG12:AG20"/>
+    <mergeCell ref="AG31:AG34"/>
+    <mergeCell ref="B31:M31"/>
+    <mergeCell ref="AA31:AA34"/>
+    <mergeCell ref="AB31:AB34"/>
+    <mergeCell ref="AC31:AC34"/>
+    <mergeCell ref="AD31:AD34"/>
+    <mergeCell ref="AE31:AE34"/>
+    <mergeCell ref="AF31:AF34"/>
+    <mergeCell ref="AG21:AG30"/>
+    <mergeCell ref="D21:H30"/>
+    <mergeCell ref="B21:B30"/>
+    <mergeCell ref="I21:M30"/>
+    <mergeCell ref="AA21:AA30"/>
+    <mergeCell ref="AB21:AB30"/>
+    <mergeCell ref="AC21:AC30"/>
+    <mergeCell ref="AD21:AD30"/>
+    <mergeCell ref="AE21:AE30"/>
+    <mergeCell ref="AF21:AF30"/>
+    <mergeCell ref="AI35:AI39"/>
+    <mergeCell ref="AI40:AI46"/>
+    <mergeCell ref="AI47:AI50"/>
+    <mergeCell ref="AI2:AI7"/>
+    <mergeCell ref="AI10:AI11"/>
+    <mergeCell ref="AI12:AI20"/>
+    <mergeCell ref="AI21:AI30"/>
+    <mergeCell ref="AI31:AI34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>

</xml_diff>